<commit_message>
Added Seychelles wildlife reports
</commit_message>
<xml_diff>
--- a/wildlife/reports/United-Kingdom/richness/2020/richness.xlsx
+++ b/wildlife/reports/United-Kingdom/richness/2020/richness.xlsx
@@ -465,10 +465,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>51.6708</v>
+        <v>51.67167</v>
       </c>
       <c r="D2" t="n">
-        <v>-1.288</v>
+        <v>-1.27833</v>
       </c>
       <c r="E2" t="n">
         <v>163</v>
@@ -734,7 +734,7 @@
         <v>53.55</v>
       </c>
       <c r="D16" t="n">
-        <v>-2.3333</v>
+        <v>-2.3277</v>
       </c>
       <c r="E16" t="n">
         <v>5</v>

</xml_diff>